<commit_message>
Updated website with recent changes
</commit_message>
<xml_diff>
--- a/uploads/Canon.xlsx
+++ b/uploads/Canon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOLFIX\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MOLFIX\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3784,7 +3784,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3819,7 +3819,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4030,8 +4030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1517"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4567,7 +4567,7 @@
         <v>206.22</v>
       </c>
       <c r="K12">
-        <v>206.22</v>
+        <v>4000000</v>
       </c>
       <c r="L12">
         <v>0</v>

</xml_diff>